<commit_message>
update ocnbgc for cmip6_cmcc_cmcc-esm2_ocnbgchem
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_ocnbgchem.xlsx
+++ b/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_ocnbgchem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-esm2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F0C5D7-F9A4-F34A-9635-9A9F82112819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33267D19-18BD-6745-919D-5FCE6D200D81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="444">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1352,6 +1352,9 @@
   </si>
   <si>
     <t>The Biogeochemical Flux Model (BFM v5.2, www.bfm-community.eu/) is a biomass-based numerical model to simulate the major biogeochemical processes occurring in pelagic, benthic and sea-ice components of marine ecosystems. The BFM considers the cycles of nitrogen, phosphorus, silica, iron, carbon, and oxygen in the water, sediments, sea ice and in the related organisms from bacteria to benthic meiofauna. All living organisms are Plankton dynamics are parameterized in terms of functional groups with prescribed functional traits. For instance, the BFM plankton functional groups are subdivided in producers (phytoplankton), consumers (zooplankton), and decomposers (bacteria). These broad functional classifications are further partitioned into functional subgroups to create a planktonic food web (e.g. diatoms, picophytoplankton, microzooplankton, etc.). A full description of model equations and available parameterizations is given in bfm_2020.</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
   </si>
 </sst>
 </file>
@@ -2006,10 +2009,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2056,72 +2059,80 @@
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>438</v>
+        <v>4</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>422</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B10" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B11" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:B20" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Tracers"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2131,7 +2142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>